<commit_message>
First few tests are ready
</commit_message>
<xml_diff>
--- a/manual_tests/Manual_tests.xlsx
+++ b/manual_tests/Manual_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sores\Desktop\Mernokinfo\IET\iet-hf-2024-i01\manual_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75513387-CF76-463B-88CB-06B1BA3BBD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334A333E-4ADE-4DF8-BA84-8002AE67FE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="110">
   <si>
     <t>Low</t>
   </si>
@@ -70,9 +70,6 @@
     <t>SCREENSHOT</t>
   </si>
   <si>
-    <t>DATE REPORTED</t>
-  </si>
-  <si>
     <t>Critical</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>Complex</t>
   </si>
   <si>
-    <t>Very Low</t>
-  </si>
-  <si>
     <t>Finished</t>
   </si>
   <si>
@@ -149,6 +143,237 @@
   </si>
   <si>
     <t>TESTED BY</t>
+  </si>
+  <si>
+    <t>barni10102</t>
+  </si>
+  <si>
+    <t>Program elindul</t>
+  </si>
+  <si>
+    <t>Le kell tesztelni, hogy a program 22-es jdk-n is elindul és működik-e mivel 18-as jdk-n lett írva</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>Néhány java függvényt át kellet írni, mert megváltozott a működésük, de azon kívül minden rendben volt</t>
+  </si>
+  <si>
+    <t>A beállításokban beállított értékek alapján kezdődik el a játék</t>
+  </si>
+  <si>
+    <t>Meg kell vizsgálni, hogy a beállításokban beállított értékek valóban helyesek, és azokkal indul a játék</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>Semmi probléma nem volt, minden helyesen inicializálódik</t>
+  </si>
+  <si>
+    <t>TEST DATE</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>test4</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>test8</t>
+  </si>
+  <si>
+    <t>test9</t>
+  </si>
+  <si>
+    <t>test10</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>test13</t>
+  </si>
+  <si>
+    <t>test14</t>
+  </si>
+  <si>
+    <t>test15</t>
+  </si>
+  <si>
+    <t>test16</t>
+  </si>
+  <si>
+    <t>test17</t>
+  </si>
+  <si>
+    <t>test18</t>
+  </si>
+  <si>
+    <t>Minden rendben volt, a szerelők mozgásával</t>
+  </si>
+  <si>
+    <t>Az első szabotőr utána sorban következnek a további szabotőrök és ők is rendesen a játék leírása alapján tudnak mozogni</t>
+  </si>
+  <si>
+    <t>Az utolsó szabotőr után következik az első szerelő, utána a további szerelők és az ő mozgásuk is rendben van</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A szabotőr játékosok a leírás alapján tudnak mozogni </t>
+  </si>
+  <si>
+    <t>Meg kell nézni, hogy a szabotőrök tudnak-e mozogni megfelelően, azaz két szabotőr nem tud egy csőre lépni, viszont egy pumpára, hegyre vagy ciszternára már igen</t>
+  </si>
+  <si>
+    <t>Minden rendben volt, a szabotőrök mozgásával</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A szerelő játékosok a leírás alapján tudnak mozogni </t>
+  </si>
+  <si>
+    <t>Meg kell nézni, hogy a szerelők tudnak-e mozogni megfelelően, azaz két szerelő nem tud egy csőre lépni, viszont egy pumpára, hegyre vagy ciszternára már igen</t>
+  </si>
+  <si>
+    <t>A szabotőrök ugyanúgy a leírás alapján tudnak mozogni, mint az első szabotőr, csak nekik várniuk kell a sorukra</t>
+  </si>
+  <si>
+    <t>Minden rendben volt, a szabotőrök a leírásnak megfelelően mozogtak</t>
+  </si>
+  <si>
+    <t>A szerelők ugyanúgy a leírás alapján tudnak mozogni, mint az első szerelő, csak nekik várniuk kell a sorukra, illetve az első szerelő az utolsó szabotőr után következik</t>
+  </si>
+  <si>
+    <t>Minden rendben volt, a szerelők a leírásnak megfelelően mozogtak, és a sorrend is megfelelő volt</t>
+  </si>
+  <si>
+    <t>Egy szerelő és egy szabotőr nem tud egyszerre egy csövön állni</t>
+  </si>
+  <si>
+    <t>Minden rendben volt a működés szempontjából, viszont játékélmény szempontjából érdekes döntés volt így implementálni</t>
+  </si>
+  <si>
+    <t>A játékban ha a víz a hegytől elfolyik a ciszternákba, akkor a szerelők kapnak pontot</t>
+  </si>
+  <si>
+    <t>A szerelők pontszáma nő, minden lépés után, ha vezet út a hegyekből a ciszternákba, és ezen az úton nincs törött cső vagy rossz pumpa</t>
+  </si>
+  <si>
+    <t>A szerelők megkapják a pontot, ha megy víz a hegyekből a ciszternákba</t>
+  </si>
+  <si>
+    <t>Ha a víz nem folyik el a hegyekig, egy lyukas cső vagy pumpa miatt, akkor a lépésben a szabotőrök kapnak pontot</t>
+  </si>
+  <si>
+    <t>A szerelők megkapják a megérdemelt pontjukat</t>
+  </si>
+  <si>
+    <t>Ha a víz nem folyik el a hegyekig, egy lyukas cső miatt, akkor a lépésben a szabotőrök kapnak pontot</t>
+  </si>
+  <si>
+    <t>Ha a víz nem folyik el a hegyekig, egy rossz pumpa miatt, akkor a lépésben a szabotőrök kapnak pontot</t>
+  </si>
+  <si>
+    <t>Meg kell várni amég egy pumpa rossz lesz</t>
+  </si>
+  <si>
+    <t>Szabotőrök pontja nő</t>
+  </si>
+  <si>
+    <t>Nem kapnak pontot a szabotőrök</t>
+  </si>
+  <si>
+    <t>A szerelőknek jóval nehezebb így pontot gyűjteniük</t>
+  </si>
+  <si>
+    <t>A szabotőrök meg tudnak rongálni egy pumpát</t>
+  </si>
+  <si>
+    <t>A szabotőrök képesek a pumpákat rongálni, ami következtében azok már nem pumpálnak vizet</t>
+  </si>
+  <si>
+    <t>A pumpa elromlik</t>
+  </si>
+  <si>
+    <t>Nem romlik el a pumpa, a rongálás művelete nem hajtódik végre, a lépés nem történik meg</t>
+  </si>
+  <si>
+    <t>Ez egy fontos része lenne a játéknak, így eléggé csökkenti a szabotőrök esélyét</t>
+  </si>
+  <si>
+    <t>A pumpák random időközönként, elromlanak</t>
+  </si>
+  <si>
+    <t>A pumpák két lépés között bármikor elromolhatnak maguktól</t>
+  </si>
+  <si>
+    <t>Minden rendben volt, a pumpák elromlanak random időközönként</t>
+  </si>
+  <si>
+    <t>A szabotőrök meg tudnak rongálni egy csövet</t>
+  </si>
+  <si>
+    <t>A szabotőrök, ha a csövön állnak és van még lépésük, akkor meg tudják rongálni a csövet, amin állnak</t>
+  </si>
+  <si>
+    <t>A csöveket a leírtak alapjánn lehet rongálni</t>
+  </si>
+  <si>
+    <t>A szerelők meg tudják javítani a kilyukasztott csövet</t>
+  </si>
+  <si>
+    <t>A szerelők, ha a kilyukasztott csövön állnak és van még lépésük, akkor be tudják foltozni a kilyukasztott csövet</t>
+  </si>
+  <si>
+    <t>A szerelők sikeresen meg tudják javítani a kilyukasztott csövet</t>
+  </si>
+  <si>
+    <t>A szerelők meg tudják javítani a rossz pumpákat</t>
+  </si>
+  <si>
+    <t>A szerelők meg tudják javítani a rossz pumpákat, ha az adott pumpán állnak és van még lépésük</t>
+  </si>
+  <si>
+    <t>A pumpa megjavítódik</t>
+  </si>
+  <si>
+    <t>Egy pumpán kell állnunk szerelőként és lennie kell lépésünknek még, ilyenkor a 6-os gombot megnyomja megszerelődik a pumpa</t>
+  </si>
+  <si>
+    <t>Néha a szerelés után a pumpa el is romlik, ezért olyan, mintha nem is szereltük volna meg a pumpát</t>
+  </si>
+  <si>
+    <t>Annyira nem vészes ez a dolog, mert tulajdonképpen a javítás megtörténik, a lépést elveszi, de azért jobb lenne, ha a rongálást követően nem tudna elromlani a pumpa</t>
+  </si>
+  <si>
+    <t>A szerelők fel tudnak venni pumpát a ciszternákon</t>
+  </si>
+  <si>
+    <t>Ha a szerelők elmennek a ciszternákra, akkor ott fel tudnak venni pumpát</t>
+  </si>
+  <si>
+    <t>A pumpán kell állni, lennie kell még lépésnek az adott körben és szabotőrnek kell lennünk, és ilyenkor meg kell nyomni a 0-s gombot</t>
+  </si>
+  <si>
+    <t>A ciszternáknál lennie kell felvehető pumpának, a ciszternákon kell lennünk és lennie kell lépésünknek, ezek után a 7-es gombal veszünk fel pumpát</t>
+  </si>
+  <si>
+    <t>Felveszünk egy pumpát</t>
+  </si>
+  <si>
+    <t>A pumpa felvétele megtörténik, de ugyanúgy, mint a 15. tesztnél, itt is tud a felvevés után újra spawnolni egy pumpa és olyan mintha nem vettük volna fel, mert a pumpák száma a ui-on nem csökken</t>
+  </si>
+  <si>
+    <t>Ugyanúgy, mint az 15.-ös tesztnél valójában az történik, amit akarunk, de zavaró lehet és érthetetlen, hogy miért nem csökken a pumpák száma</t>
   </si>
 </sst>
 </file>
@@ -159,7 +384,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +457,14 @@
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -419,12 +652,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -495,6 +729,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -543,44 +807,18 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hivatkozás" xfId="3" builtinId="8"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Pénznem" xfId="1" builtinId="4"/>
@@ -1469,7 +1707,7 @@
     <tableColumn id="1" xr3:uid="{60DB6528-7C6F-3949-8DC5-39029C2B8FA9}" name="ID" dataDxfId="32"/>
     <tableColumn id="2" xr3:uid="{DBAAE93F-9BEF-7D4F-B744-E9172B23F1A6}" name="TITLE" dataDxfId="31"/>
     <tableColumn id="3" xr3:uid="{F2308639-C083-2440-A774-5C1BA0C1C549}" name="TESTED BY" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{35B302BC-E331-C84C-AC2F-408914E97D36}" name="DATE REPORTED" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{35B302BC-E331-C84C-AC2F-408914E97D36}" name="TEST DATE" dataDxfId="29"/>
     <tableColumn id="5" xr3:uid="{4747DC13-4CC3-FE47-BD01-EBE151C2885A}" name="SUMMARY" dataDxfId="28"/>
     <tableColumn id="9" xr3:uid="{45E0605B-7673-40BB-90D8-5D705B56C09F}" name="Complexity" dataDxfId="27"/>
     <tableColumn id="15" xr3:uid="{4D724BBC-C07C-B64B-9635-FFC079012231}" name="BUG OCCURED" dataDxfId="26"/>
@@ -1755,9 +1993,9 @@
   </sheetPr>
   <dimension ref="B1:AD57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1786,7 +2024,7 @@
   <sheetData>
     <row r="1" spans="2:30" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="3"/>
@@ -1807,54 +2045,54 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="44" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="45"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="27"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="30"/>
       <c r="P2" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V2" s="25"/>
     </row>
     <row r="3" spans="2:30" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="17" t="s">
         <v>3</v>
@@ -1866,366 +2104,726 @@
         <v>1</v>
       </c>
       <c r="L3" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="17" t="s">
-        <v>13</v>
-      </c>
       <c r="N3" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="T3" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U3" s="25"/>
-      <c r="V3" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="W3" s="49"/>
-      <c r="X3" s="50"/>
+      <c r="V3" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" s="32"/>
+      <c r="X3" s="33"/>
       <c r="Y3" s="25"/>
-      <c r="Z3" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA3" s="37"/>
+      <c r="Z3" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA3" s="47"/>
       <c r="AB3" s="25"/>
-      <c r="AC3" s="28" t="s">
+      <c r="AC3" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AD3" s="29"/>
-    </row>
-    <row r="4" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="AD3" s="39"/>
+    </row>
+    <row r="4" spans="2:30" ht="54" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="15">
+        <v>45428</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="52" t="s">
+        <v>36</v>
+      </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="O4" s="9"/>
-      <c r="P4" s="19"/>
+      <c r="P4" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="R4" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="U4" s="25"/>
+      <c r="V4" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="35"/>
+      <c r="X4" s="35"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD4" s="37"/>
+    </row>
+    <row r="5" spans="2:30" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="15">
+        <v>45428</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="25"/>
-      <c r="V4" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="W4" s="52"/>
-      <c r="X4" s="52"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="26" t="s">
+      <c r="I5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD4" s="27"/>
-    </row>
-    <row r="5" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="J5" s="52" t="s">
+        <v>40</v>
+      </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="19"/>
+      <c r="P5" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="R5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="T5" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U5" s="25"/>
-      <c r="V5" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
+      <c r="V5" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="W5" s="45"/>
+      <c r="X5" s="45"/>
       <c r="Y5" s="25"/>
-      <c r="Z5" s="38" t="s">
+      <c r="Z5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="AA5" s="39"/>
+      <c r="AA5" s="49"/>
       <c r="AB5" s="25"/>
-      <c r="AC5" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD5" s="31"/>
-    </row>
-    <row r="6" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="AC5" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD5" s="41"/>
+    </row>
+    <row r="6" spans="2:30" ht="108" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="15">
+        <v>45428</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="52" t="s">
+        <v>43</v>
+      </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="O6" s="9"/>
-      <c r="P6" s="19"/>
+      <c r="P6" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="R6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="40" t="s">
+      <c r="Z6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="AA6" s="41"/>
-      <c r="AC6" s="32" t="s">
+      <c r="AA6" s="51"/>
+      <c r="AC6" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD6" s="43"/>
+    </row>
+    <row r="7" spans="2:30" ht="108" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AD6" s="33"/>
-    </row>
-    <row r="7" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="E7" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="52" t="s">
+        <v>44</v>
+      </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="O7" s="9"/>
-      <c r="P7" s="19"/>
+      <c r="P7" s="19" t="s">
+        <v>58</v>
+      </c>
       <c r="R7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="U7" s="25"/>
       <c r="Y7" s="25"/>
-      <c r="Z7" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA7" s="43"/>
       <c r="AB7" s="25"/>
     </row>
-    <row r="8" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+    <row r="8" spans="2:30" ht="81" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="52" t="s">
+        <v>45</v>
+      </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="O8" s="9"/>
-      <c r="P8" s="19"/>
-    </row>
-    <row r="9" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="P8" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" ht="108" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="52" t="s">
+        <v>46</v>
+      </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="O9" s="9"/>
-      <c r="P9" s="19"/>
-    </row>
-    <row r="10" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="P9" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" ht="54" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
+        <v>7</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="54">
+        <v>45429</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>47</v>
+      </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="O10" s="9"/>
-      <c r="P10" s="19"/>
-    </row>
-    <row r="11" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="P10" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" ht="81" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="52" t="s">
+        <v>48</v>
+      </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="O11" s="9"/>
-      <c r="P11" s="19"/>
-    </row>
-    <row r="12" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="P11" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" ht="81" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="52" t="s">
+        <v>49</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="O12" s="9"/>
-      <c r="P12" s="19"/>
-    </row>
-    <row r="13" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="19"/>
-    </row>
-    <row r="14" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="19"/>
-    </row>
-    <row r="15" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="P12" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
+        <v>10</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="N13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" ht="81" x14ac:dyDescent="0.25">
+      <c r="B14" s="12">
+        <v>11</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="N14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P14" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
+        <v>12</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="O15" s="9"/>
-      <c r="P15" s="19"/>
-    </row>
-    <row r="16" spans="2:30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="P15" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="12">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="52" t="s">
+        <v>52</v>
+      </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="O16" s="9"/>
-      <c r="P16" s="19"/>
-    </row>
-    <row r="17" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
+      <c r="P16" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="81" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
+        <v>14</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="52" t="s">
+        <v>53</v>
+      </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="O17" s="9"/>
-      <c r="P17" s="19"/>
-    </row>
-    <row r="18" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="19"/>
-    </row>
-    <row r="19" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="19"/>
-    </row>
-    <row r="20" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
+      <c r="P17" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="81" x14ac:dyDescent="0.25">
+      <c r="B18" s="12">
+        <v>15</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="N18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="135" x14ac:dyDescent="0.25">
+      <c r="B19" s="12">
+        <v>16</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="15">
+        <v>45429</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="12">
+        <v>17</v>
+      </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="15"/>
@@ -2233,15 +2831,19 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
+      <c r="J20" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="O20" s="9"/>
       <c r="P20" s="19"/>
     </row>
-    <row r="21" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="12">
+        <v>18</v>
+      </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="15"/>
@@ -2249,14 +2851,16 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
+      <c r="J21" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="19"/>
     </row>
-    <row r="22" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -2272,7 +2876,7 @@
       <c r="O22" s="9"/>
       <c r="P22" s="19"/>
     </row>
-    <row r="23" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="12"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -2288,7 +2892,7 @@
       <c r="O23" s="9"/>
       <c r="P23" s="19"/>
     </row>
-    <row r="24" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="12"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -2304,7 +2908,7 @@
       <c r="O24" s="9"/>
       <c r="P24" s="19"/>
     </row>
-    <row r="25" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="12"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2320,7 +2924,7 @@
       <c r="O25" s="9"/>
       <c r="P25" s="19"/>
     </row>
-    <row r="26" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="12"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -2336,7 +2940,7 @@
       <c r="O26" s="9"/>
       <c r="P26" s="19"/>
     </row>
-    <row r="27" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="12"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2352,7 +2956,7 @@
       <c r="O27" s="9"/>
       <c r="P27" s="19"/>
     </row>
-    <row r="28" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="12"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -2368,7 +2972,7 @@
       <c r="O28" s="9"/>
       <c r="P28" s="19"/>
     </row>
-    <row r="29" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -2384,7 +2988,7 @@
       <c r="O29" s="9"/>
       <c r="P29" s="19"/>
     </row>
-    <row r="30" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="12"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -2400,7 +3004,7 @@
       <c r="O30" s="9"/>
       <c r="P30" s="19"/>
     </row>
-    <row r="31" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -2416,7 +3020,7 @@
       <c r="O31" s="9"/>
       <c r="P31" s="19"/>
     </row>
-    <row r="32" spans="2:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="12"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -2432,7 +3036,7 @@
       <c r="O32" s="9"/>
       <c r="P32" s="19"/>
     </row>
-    <row r="33" spans="2:24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
@@ -2448,7 +3052,7 @@
       <c r="O33" s="14"/>
       <c r="P33" s="20"/>
     </row>
-    <row r="34" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B34" s="13"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2464,7 +3068,7 @@
       <c r="O34" s="9"/>
       <c r="P34" s="19"/>
     </row>
-    <row r="35" spans="2:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B35" s="13"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -2480,7 +3084,7 @@
       <c r="O35" s="9"/>
       <c r="P35" s="19"/>
     </row>
-    <row r="36" spans="2:24" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B36" s="13"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -2496,7 +3100,7 @@
       <c r="O36" s="9"/>
       <c r="P36" s="19"/>
     </row>
-    <row r="37" spans="2:24" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" s="13"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
@@ -2512,7 +3116,7 @@
       <c r="O37" s="9"/>
       <c r="P37" s="19"/>
     </row>
-    <row r="38" spans="2:24" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B38" s="13"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -2544,7 +3148,7 @@
       <c r="O39" s="9"/>
       <c r="P39" s="19"/>
     </row>
-    <row r="40" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B40" s="12"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
@@ -2560,7 +3164,7 @@
       <c r="O40" s="9"/>
       <c r="P40" s="19"/>
     </row>
-    <row r="41" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B41" s="12"/>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -2645,7 +3249,7 @@
       <c r="P45" s="19"/>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
@@ -2661,7 +3265,7 @@
       <c r="O46" s="9"/>
       <c r="P46" s="19"/>
     </row>
-    <row r="47" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -2677,7 +3281,7 @@
       <c r="O47" s="9"/>
       <c r="P47" s="19"/>
     </row>
-    <row r="48" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -2693,7 +3297,7 @@
       <c r="O48" s="9"/>
       <c r="P48" s="19"/>
     </row>
-    <row r="49" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -2844,14 +3448,7 @@
       <c r="P57" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="V4:X4"/>
+  <mergeCells count="15">
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="AC5:AD5"/>
@@ -2861,6 +3458,12 @@
     <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="Z5:AA5"/>
     <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="V4:X4"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="N4:N1048576">
@@ -2940,16 +3543,33 @@
       <formula1>$V$4:$V$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G1048576" xr:uid="{D87E531E-F776-4754-8948-972B264FA031}">
-      <formula1>$Z$4:$Z$7</formula1>
+      <formula1>$Z$4:$Z$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I1048576" xr:uid="{ED3ACD48-5CBD-44BB-ADE6-D38BE45ED69F}">
       <formula1>$AC$4:$AC$6</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1" display="/manual_tests/images/1.png" xr:uid="{07BA4BC4-4123-4660-83BF-772535788EA1}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{E96E6A2D-3CF6-4DC8-AD1E-37F086528B18}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{B079A5BE-355B-4FE9-A967-3EB7E15080A1}"/>
+    <hyperlink ref="J7" r:id="rId4" xr:uid="{A705FC68-FB08-4AD5-BFAC-9473B25122C0}"/>
+    <hyperlink ref="J8" r:id="rId5" xr:uid="{0BFE5A7F-A8A9-4480-836B-7832ECD9A467}"/>
+    <hyperlink ref="J9" r:id="rId6" xr:uid="{0B1283E1-130C-4A7E-B667-CB0EFFCB1318}"/>
+    <hyperlink ref="J10" r:id="rId7" xr:uid="{ED845BAF-C8E9-43A6-9B67-C2A4B759D08D}"/>
+    <hyperlink ref="J11" r:id="rId8" xr:uid="{2DBCFAAC-6C67-4FA3-96DC-E13C97AF40D9}"/>
+    <hyperlink ref="J12" r:id="rId9" xr:uid="{A1A8BDAD-15D8-410F-B9AB-E8933CFBBC7F}"/>
+    <hyperlink ref="J13" r:id="rId10" xr:uid="{364AC713-65EB-48ED-9950-4FAEBFD22E8A}"/>
+    <hyperlink ref="J14" r:id="rId11" xr:uid="{D3CDEA50-92C4-4EA8-B475-715C6B613B30}"/>
+    <hyperlink ref="J16" r:id="rId12" xr:uid="{081DDA5A-4FE4-42BE-B85B-253E967FB026}"/>
+    <hyperlink ref="J17" r:id="rId13" xr:uid="{F33010DB-3E0A-4319-A6B8-AB3D0D266D16}"/>
+    <hyperlink ref="J18" r:id="rId14" xr:uid="{90C18DAE-0744-4B87-A9F2-561D81B15469}"/>
+    <hyperlink ref="J19" r:id="rId15" xr:uid="{9520F7F9-97BF-4C2B-BF92-33ECE114FE64}"/>
+  </hyperlinks>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="44" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="44" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Summary and nextInt boundary fix
</commit_message>
<xml_diff>
--- a/manual_tests/Manual_tests.xlsx
+++ b/manual_tests/Manual_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sores\Desktop\Mernokinfo\IET\iet-hf-2024-i01\manual_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D376A022-AE5D-417F-92F3-8E60B255CAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0A13E8-BBC3-4F41-834D-309BDD4D474E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -954,6 +954,36 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -972,61 +1002,31 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1036,35 +1036,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Pénznem" xfId="1" builtinId="4"/>
   </cellStyles>
-  <dxfs count="88">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="39">
     <dxf>
       <fill>
         <patternFill>
@@ -1199,321 +1171,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAEEF3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2248,23 +1905,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7FE54C03-3649-1248-A4BA-0578B3EB9A73}" name="Table1" displayName="Table1" ref="B3:P57" totalsRowShown="0" headerRowDxfId="87" dataDxfId="85" headerRowBorderDxfId="86" tableBorderDxfId="84" totalsRowBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7FE54C03-3649-1248-A4BA-0578B3EB9A73}" name="Table1" displayName="Table1" ref="B3:P57" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{60DB6528-7C6F-3949-8DC5-39029C2B8FA9}" name="ID" dataDxfId="82"/>
-    <tableColumn id="2" xr3:uid="{DBAAE93F-9BEF-7D4F-B744-E9172B23F1A6}" name="TITLE" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{F2308639-C083-2440-A774-5C1BA0C1C549}" name="TESTED BY" dataDxfId="80"/>
-    <tableColumn id="4" xr3:uid="{35B302BC-E331-C84C-AC2F-408914E97D36}" name="TEST DATE" dataDxfId="79"/>
-    <tableColumn id="5" xr3:uid="{4747DC13-4CC3-FE47-BD01-EBE151C2885A}" name="SUMMARY" dataDxfId="78"/>
-    <tableColumn id="9" xr3:uid="{45E0605B-7673-40BB-90D8-5D705B56C09F}" name="Complexity" dataDxfId="77"/>
-    <tableColumn id="15" xr3:uid="{4D724BBC-C07C-B64B-9635-FFC079012231}" name="BUG OCCURED" dataDxfId="76"/>
-    <tableColumn id="10" xr3:uid="{506D8D17-AE26-470F-915C-DC3ACB652038}" name="STATUS" dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{46C8A186-CFD5-1A4D-9007-10EAF4DABC90}" name="SCREENSHOT" dataDxfId="74"/>
-    <tableColumn id="16" xr3:uid="{C8C5A442-59A6-7F47-912F-90E528C44DD0}" name="STEPS TO REPRODUCE" dataDxfId="73"/>
-    <tableColumn id="17" xr3:uid="{A5486FF8-AB31-4345-BCB0-8D9DF0FD699A}" name="EXPECTED RESULT" dataDxfId="72"/>
-    <tableColumn id="18" xr3:uid="{39C591F4-782F-CB4B-BF44-B4CCD11723A9}" name="ACTUAL RESULT" dataDxfId="71"/>
-    <tableColumn id="19" xr3:uid="{88C11E58-C0F8-7343-95E5-7CE29CFDEE15}" name="PRIORITY" dataDxfId="70"/>
-    <tableColumn id="20" xr3:uid="{8A5D5C17-B27D-7A42-B45A-2EC555DE51B0}" name="IMPAIRS THE USER EXPERIENCE" dataDxfId="69"/>
-    <tableColumn id="14" xr3:uid="{FC984278-8598-8C42-AD4C-1547465D297D}" name="NOTES ABOUT THE TEST" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{60DB6528-7C6F-3949-8DC5-39029C2B8FA9}" name="ID" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{DBAAE93F-9BEF-7D4F-B744-E9172B23F1A6}" name="TITLE" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{F2308639-C083-2440-A774-5C1BA0C1C549}" name="TESTED BY" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{35B302BC-E331-C84C-AC2F-408914E97D36}" name="TEST DATE" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{4747DC13-4CC3-FE47-BD01-EBE151C2885A}" name="SUMMARY" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{45E0605B-7673-40BB-90D8-5D705B56C09F}" name="Complexity" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{4D724BBC-C07C-B64B-9635-FFC079012231}" name="BUG OCCURED" dataDxfId="27"/>
+    <tableColumn id="10" xr3:uid="{506D8D17-AE26-470F-915C-DC3ACB652038}" name="STATUS" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{46C8A186-CFD5-1A4D-9007-10EAF4DABC90}" name="SCREENSHOT" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{C8C5A442-59A6-7F47-912F-90E528C44DD0}" name="STEPS TO REPRODUCE" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{A5486FF8-AB31-4345-BCB0-8D9DF0FD699A}" name="EXPECTED RESULT" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{39C591F4-782F-CB4B-BF44-B4CCD11723A9}" name="ACTUAL RESULT" dataDxfId="22"/>
+    <tableColumn id="19" xr3:uid="{88C11E58-C0F8-7343-95E5-7CE29CFDEE15}" name="PRIORITY" dataDxfId="21"/>
+    <tableColumn id="20" xr3:uid="{8A5D5C17-B27D-7A42-B45A-2EC555DE51B0}" name="IMPAIRS THE USER EXPERIENCE" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{FC984278-8598-8C42-AD4C-1547465D297D}" name="NOTES ABOUT THE TEST" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2540,7 +2197,7 @@
   <dimension ref="B1:AD57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2591,28 +2248,28 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="2:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="39" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="37" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39" t="s">
+      <c r="L2" s="27"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="40"/>
+      <c r="O2" s="30"/>
       <c r="P2" s="20" t="s">
         <v>13</v>
       </c>
@@ -2671,21 +2328,21 @@
         <v>19</v>
       </c>
       <c r="U3" s="22"/>
-      <c r="V3" s="41" t="s">
+      <c r="V3" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="W3" s="42"/>
-      <c r="X3" s="43"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="33"/>
       <c r="Y3" s="22"/>
-      <c r="Z3" s="32" t="s">
+      <c r="Z3" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="33"/>
+      <c r="AA3" s="44"/>
       <c r="AB3" s="22"/>
-      <c r="AC3" s="26" t="s">
+      <c r="AC3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="AD3" s="27"/>
+      <c r="AD3" s="37"/>
     </row>
     <row r="4" spans="2:30" ht="54" x14ac:dyDescent="0.25">
       <c r="B4" s="9">
@@ -2729,21 +2386,21 @@
         <v>20</v>
       </c>
       <c r="U4" s="22"/>
-      <c r="V4" s="30" t="s">
+      <c r="V4" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
       <c r="Y4" s="22"/>
-      <c r="Z4" s="24" t="s">
+      <c r="Z4" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="AA4" s="25"/>
+      <c r="AA4" s="35"/>
       <c r="AB4" s="22"/>
-      <c r="AC4" s="24" t="s">
+      <c r="AC4" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="AD4" s="25"/>
+      <c r="AD4" s="35"/>
     </row>
     <row r="5" spans="2:30" ht="67.5" x14ac:dyDescent="0.25">
       <c r="B5" s="9">
@@ -2783,25 +2440,25 @@
       <c r="R5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="T5" s="44" t="s">
+      <c r="T5" s="24" t="s">
         <v>21</v>
       </c>
       <c r="U5" s="22"/>
-      <c r="V5" s="46" t="s">
+      <c r="V5" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="47"/>
-      <c r="X5" s="48"/>
+      <c r="W5" s="42"/>
+      <c r="X5" s="41"/>
       <c r="Y5" s="22"/>
-      <c r="Z5" s="34" t="s">
+      <c r="Z5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="AA5" s="35"/>
+      <c r="AA5" s="46"/>
       <c r="AB5" s="22"/>
-      <c r="AC5" s="28" t="s">
+      <c r="AC5" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="AD5" s="29"/>
+      <c r="AD5" s="39"/>
     </row>
     <row r="6" spans="2:30" ht="108" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
@@ -2838,17 +2495,17 @@
       <c r="P6" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="R6" s="45" t="s">
+      <c r="R6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="46" t="s">
+      <c r="Z6" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="AA6" s="48"/>
-      <c r="AC6" s="46" t="s">
+      <c r="AA6" s="41"/>
+      <c r="AC6" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="AD6" s="48"/>
+      <c r="AD6" s="41"/>
     </row>
     <row r="7" spans="2:30" ht="108" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
@@ -2885,7 +2542,7 @@
       <c r="P7" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="R7" s="44" t="s">
+      <c r="R7" s="24" t="s">
         <v>0</v>
       </c>
       <c r="U7" s="22"/>
@@ -4461,11 +4118,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="V3:X3"/>
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="AC5:AD5"/>
@@ -4476,88 +4128,82 @@
     <mergeCell ref="Z5:AA5"/>
     <mergeCell ref="Z6:AA6"/>
     <mergeCell ref="V4:X4"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="V3:X3"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="H4:H1048576">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",H4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N4:N1048576">
-    <cfRule type="containsText" dxfId="43" priority="32" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="17" priority="32" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",N4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="33" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="16" priority="33" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",N4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="34" operator="containsText" text="Critical">
+    <cfRule type="containsText" dxfId="15" priority="34" operator="containsText" text="Critical">
       <formula>NOT(ISERROR(SEARCH("Critical",N4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:R6">
-    <cfRule type="containsText" dxfId="40" priority="29" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="14" priority="29" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",R4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="30" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="13" priority="30" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",R4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="31" operator="containsText" text="Showstopper">
+    <cfRule type="containsText" dxfId="12" priority="31" operator="containsText" text="Showstopper">
       <formula>NOT(ISERROR(SEARCH("Showstopper",R4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4">
-    <cfRule type="containsText" dxfId="37" priority="23" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="11" priority="23" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="24" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="10" priority="24" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",T4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="25" operator="containsText" text="Showstopper">
+    <cfRule type="containsText" dxfId="9" priority="25" operator="containsText" text="Showstopper">
       <formula>NOT(ISERROR(SEARCH("Showstopper",T4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4">
-    <cfRule type="containsText" dxfId="34" priority="20" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="8" priority="20" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",V4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="21" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="7" priority="21" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",V4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="22" operator="containsText" text="Showstopper">
+    <cfRule type="containsText" dxfId="6" priority="22" operator="containsText" text="Showstopper">
       <formula>NOT(ISERROR(SEARCH("Showstopper",V4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z4">
-    <cfRule type="containsText" dxfId="31" priority="11" operator="containsText" text="Minor">
+  <conditionalFormatting sqref="Z4:Z5">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",Z4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="12" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",Z4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="13" operator="containsText" text="Showstopper">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Showstopper">
       <formula>NOT(ISERROR(SEARCH("Showstopper",Z4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC4:AC5">
-    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",AC4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="6" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",AC4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="7" operator="containsText" text="Showstopper">
+    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="Showstopper">
       <formula>NOT(ISERROR(SEARCH("Showstopper",AC4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z5">
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="Minor">
-      <formula>NOT(ISERROR(SEARCH("Minor",Z5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="Major">
-      <formula>NOT(ISERROR(SEARCH("Major",Z5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="Showstopper">
-      <formula>NOT(ISERROR(SEARCH("Showstopper",Z5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H1048576">
-    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">

</xml_diff>